<commit_message>
Fixing ImportAbsencesDriver Pair programmed with @Bsvrd
</commit_message>
<xml_diff>
--- a/workbook/workbook.xlsx
+++ b/workbook/workbook.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="21"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Week 1" sheetId="1" state="visible" r:id="rId2"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="47">
   <si>
     <t>Monday</t>
   </si>
@@ -76,10 +76,16 @@
     <t>X</t>
   </si>
   <si>
+    <t>S5</t>
+  </si>
+  <si>
     <t>BD</t>
   </si>
   <si>
     <t>BS</t>
+  </si>
+  <si>
+    <t>S3</t>
   </si>
   <si>
     <t>OM</t>
@@ -118,13 +124,7 @@
     <t>S2</t>
   </si>
   <si>
-    <t>S3</t>
-  </si>
-  <si>
     <t>S4</t>
-  </si>
-  <si>
-    <t>S5</t>
   </si>
   <si>
     <t>S6</t>
@@ -306,13 +306,14 @@
   </sheetPr>
   <dimension ref="A1:AE29"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AK15" activeCellId="0" sqref="AK15"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AJ12" activeCellId="0" sqref="AJ12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="29" min="1" style="0" width="3.51020408163265"/>
+    <col collapsed="false" hidden="false" max="1025" min="30" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -541,7 +542,9 @@
       <c r="O5" s="4"/>
       <c r="P5" s="4"/>
       <c r="Q5" s="4"/>
-      <c r="R5" s="4"/>
+      <c r="R5" s="4" t="s">
+        <v>11</v>
+      </c>
       <c r="S5" s="4"/>
       <c r="T5" s="4"/>
       <c r="U5" s="4" t="s">
@@ -563,7 +566,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -600,7 +603,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
@@ -610,7 +613,9 @@
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
-      <c r="K7" s="4"/>
+      <c r="K7" s="4" t="s">
+        <v>14</v>
+      </c>
       <c r="L7" s="4"/>
       <c r="M7" s="4" t="s">
         <v>10</v>
@@ -641,7 +646,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
@@ -682,7 +687,7 @@
         <v>5</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
@@ -1471,12 +1476,13 @@
   <dimension ref="A1:AC29"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AD1" activeCellId="0" sqref="AD1"/>
+      <selection pane="topLeft" activeCell="AG19" activeCellId="0" sqref="AG19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="29" min="1" style="0" width="3.51020408163265"/>
+    <col collapsed="false" hidden="false" max="1025" min="30" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1678,7 +1684,9 @@
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
-      <c r="E5" s="4"/>
+      <c r="E5" s="4" t="s">
+        <v>10</v>
+      </c>
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
@@ -1709,7 +1717,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -1744,7 +1752,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
@@ -1779,7 +1787,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
@@ -1814,7 +1822,7 @@
         <v>5</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
@@ -2565,6 +2573,7 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="29" min="1" style="0" width="3.51020408163265"/>
+    <col collapsed="false" hidden="false" max="1025" min="30" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2797,7 +2806,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -2832,7 +2841,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
@@ -2867,7 +2876,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
@@ -2902,7 +2911,7 @@
         <v>5</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
@@ -3653,6 +3662,7 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="29" min="1" style="0" width="3.51020408163265"/>
+    <col collapsed="false" hidden="false" max="1025" min="30" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3885,7 +3895,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -3920,7 +3930,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
@@ -3955,7 +3965,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
@@ -3990,7 +4000,7 @@
         <v>5</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
@@ -4741,6 +4751,7 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="29" min="1" style="0" width="3.51020408163265"/>
+    <col collapsed="false" hidden="false" max="1025" min="30" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4973,7 +4984,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -5008,7 +5019,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
@@ -5043,7 +5054,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
@@ -5078,7 +5089,7 @@
         <v>5</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
@@ -5829,6 +5840,7 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="29" min="1" style="0" width="3.51020408163265"/>
+    <col collapsed="false" hidden="false" max="1025" min="30" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6061,7 +6073,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -6096,7 +6108,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
@@ -6131,7 +6143,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
@@ -6166,7 +6178,7 @@
         <v>5</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
@@ -6917,6 +6929,7 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="29" min="1" style="0" width="3.51020408163265"/>
+    <col collapsed="false" hidden="false" max="1025" min="30" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7149,7 +7162,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -7184,7 +7197,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
@@ -7219,7 +7232,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
@@ -7254,7 +7267,7 @@
         <v>5</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
@@ -8005,6 +8018,7 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="29" min="1" style="0" width="3.51020408163265"/>
+    <col collapsed="false" hidden="false" max="1025" min="30" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8237,7 +8251,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -8272,7 +8286,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
@@ -8307,7 +8321,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
@@ -8342,7 +8356,7 @@
         <v>5</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
@@ -9093,6 +9107,7 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="29" min="1" style="0" width="3.51020408163265"/>
+    <col collapsed="false" hidden="false" max="1025" min="30" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9325,7 +9340,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -9360,7 +9375,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
@@ -9395,7 +9410,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
@@ -9430,7 +9445,7 @@
         <v>5</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
@@ -10181,6 +10196,7 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="29" min="1" style="0" width="3.51020408163265"/>
+    <col collapsed="false" hidden="false" max="1025" min="30" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10413,7 +10429,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -10448,7 +10464,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
@@ -10483,7 +10499,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
@@ -10518,7 +10534,7 @@
         <v>5</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
@@ -11269,6 +11285,7 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="29" min="1" style="0" width="3.51020408163265"/>
+    <col collapsed="false" hidden="false" max="1025" min="30" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11501,7 +11518,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -11536,7 +11553,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
@@ -11571,7 +11588,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
@@ -11606,7 +11623,7 @@
         <v>5</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
@@ -12357,6 +12374,7 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="29" min="1" style="0" width="3.51020408163265"/>
+    <col collapsed="false" hidden="false" max="1025" min="30" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12589,7 +12607,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -12624,7 +12642,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
@@ -12659,7 +12677,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
@@ -12694,7 +12712,7 @@
         <v>5</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
@@ -13445,6 +13463,7 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="29" min="1" style="0" width="3.51020408163265"/>
+    <col collapsed="false" hidden="false" max="1025" min="30" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13677,7 +13696,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -13712,7 +13731,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
@@ -13747,7 +13766,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
@@ -13782,7 +13801,7 @@
         <v>5</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
@@ -14531,31 +14550,34 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B1" s="0" t="s">
         <v>6</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -14576,64 +14598,64 @@
   </sheetPr>
   <dimension ref="A1:Z25"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="Y1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AA7" activeCellId="0" sqref="AA7"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Y2" activeCellId="0" sqref="Y2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.0714285714286"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C1" s="6"/>
       <c r="Y1" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="Z1" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
       <c r="Y2" s="0" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B3" s="6"/>
       <c r="C3" s="6"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
@@ -14817,12 +14839,13 @@
   <dimension ref="A1:AC29"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AD1" activeCellId="0" sqref="AD1"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="29" min="1" style="0" width="3.51020408163265"/>
+    <col collapsed="false" hidden="false" max="1025" min="30" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15059,7 +15082,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -15094,7 +15117,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
@@ -15129,7 +15152,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
@@ -15168,7 +15191,7 @@
         <v>5</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
@@ -15923,6 +15946,7 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="29" min="1" style="0" width="3.51020408163265"/>
+    <col collapsed="false" hidden="false" max="1025" min="30" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16155,7 +16179,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -16190,7 +16214,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
@@ -16225,7 +16249,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
@@ -16260,7 +16284,7 @@
         <v>5</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
@@ -17011,6 +17035,7 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="29" min="1" style="0" width="3.51020408163265"/>
+    <col collapsed="false" hidden="false" max="1025" min="30" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17243,7 +17268,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -17278,7 +17303,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
@@ -17313,7 +17338,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
@@ -17348,7 +17373,7 @@
         <v>5</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
@@ -18099,6 +18124,7 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="29" min="1" style="0" width="3.51020408163265"/>
+    <col collapsed="false" hidden="false" max="1025" min="30" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18331,7 +18357,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -18366,7 +18392,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
@@ -18401,7 +18427,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
@@ -18436,7 +18462,7 @@
         <v>5</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
@@ -19187,6 +19213,7 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="29" min="1" style="0" width="3.51020408163265"/>
+    <col collapsed="false" hidden="false" max="1025" min="30" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19407,7 +19434,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -19442,7 +19469,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
@@ -19477,7 +19504,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
@@ -19512,7 +19539,7 @@
         <v>5</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
@@ -20262,6 +20289,7 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="29" min="1" style="0" width="3.51020408163265"/>
+    <col collapsed="false" hidden="false" max="1025" min="30" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20494,7 +20522,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -20529,7 +20557,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
@@ -20564,7 +20592,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
@@ -20599,7 +20627,7 @@
         <v>5</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
@@ -21350,6 +21378,7 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="29" min="1" style="0" width="3.51020408163265"/>
+    <col collapsed="false" hidden="false" max="1025" min="30" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21677,7 +21706,7 @@
         <v>2</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
@@ -21712,7 +21741,7 @@
         <v>3</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
@@ -21747,7 +21776,7 @@
         <v>4</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
@@ -21782,7 +21811,7 @@
         <v>5</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>

</xml_diff>

<commit_message>
Big commit - Groundwork for assignment algorithm Pair programming with @tumugh
</commit_message>
<xml_diff>
--- a/workbook/workbook.xlsx
+++ b/workbook/workbook.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="21"/>
   </bookViews>
   <sheets>
     <sheet name="Week 1" sheetId="1" state="visible" r:id="rId2"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="37">
   <si>
     <t>Monday</t>
   </si>
@@ -97,9 +97,6 @@
     <t>I.D.</t>
   </si>
   <si>
-    <t>Skills</t>
-  </si>
-  <si>
     <t>Period 1</t>
   </si>
   <si>
@@ -115,73 +112,46 @@
     <t>Period 4</t>
   </si>
   <si>
+    <t>MATH</t>
+  </si>
+  <si>
+    <t>LUNCH</t>
+  </si>
+  <si>
+    <t>FREE</t>
+  </si>
+  <si>
+    <t>FIN</t>
+  </si>
+  <si>
+    <t>SCI</t>
+  </si>
+  <si>
+    <t>ART</t>
+  </si>
+  <si>
     <t>Supply Teachers</t>
   </si>
   <si>
     <t>S1</t>
   </si>
   <si>
+    <t>AB</t>
+  </si>
+  <si>
     <t>S2</t>
+  </si>
+  <si>
+    <t>CD</t>
+  </si>
+  <si>
+    <t>EF</t>
   </si>
   <si>
     <t>S4</t>
   </si>
   <si>
-    <t>S6</t>
-  </si>
-  <si>
-    <t>S7</t>
-  </si>
-  <si>
-    <t>S8</t>
-  </si>
-  <si>
-    <t>S9</t>
-  </si>
-  <si>
-    <t>S10</t>
-  </si>
-  <si>
-    <t>S11</t>
-  </si>
-  <si>
-    <t>S12</t>
-  </si>
-  <si>
-    <t>S13</t>
-  </si>
-  <si>
-    <t>S14</t>
-  </si>
-  <si>
-    <t>S15</t>
-  </si>
-  <si>
-    <t>S16</t>
-  </si>
-  <si>
-    <t>S17</t>
-  </si>
-  <si>
-    <t>S18</t>
-  </si>
-  <si>
-    <t>S19</t>
-  </si>
-  <si>
-    <t>S20</t>
-  </si>
-  <si>
-    <t>S21</t>
-  </si>
-  <si>
-    <t>S22</t>
-  </si>
-  <si>
-    <t>S23</t>
-  </si>
-  <si>
-    <t>S24</t>
+    <t>GH</t>
   </si>
 </sst>
 </file>
@@ -306,14 +276,13 @@
   </sheetPr>
   <dimension ref="A1:AE29"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AJ12" activeCellId="0" sqref="AJ12"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="29" min="1" style="0" width="3.51020408163265"/>
-    <col collapsed="false" hidden="false" max="1025" min="30" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1482,7 +1451,6 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="29" min="1" style="0" width="3.51020408163265"/>
-    <col collapsed="false" hidden="false" max="1025" min="30" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2573,7 +2541,6 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="29" min="1" style="0" width="3.51020408163265"/>
-    <col collapsed="false" hidden="false" max="1025" min="30" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3662,7 +3629,6 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="29" min="1" style="0" width="3.51020408163265"/>
-    <col collapsed="false" hidden="false" max="1025" min="30" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4751,7 +4717,6 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="29" min="1" style="0" width="3.51020408163265"/>
-    <col collapsed="false" hidden="false" max="1025" min="30" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5840,7 +5805,6 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="29" min="1" style="0" width="3.51020408163265"/>
-    <col collapsed="false" hidden="false" max="1025" min="30" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6929,7 +6893,6 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="29" min="1" style="0" width="3.51020408163265"/>
-    <col collapsed="false" hidden="false" max="1025" min="30" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8018,7 +7981,6 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="29" min="1" style="0" width="3.51020408163265"/>
-    <col collapsed="false" hidden="false" max="1025" min="30" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9107,7 +9069,6 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="29" min="1" style="0" width="3.51020408163265"/>
-    <col collapsed="false" hidden="false" max="1025" min="30" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10196,7 +10157,6 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="29" min="1" style="0" width="3.51020408163265"/>
-    <col collapsed="false" hidden="false" max="1025" min="30" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11285,7 +11245,6 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="29" min="1" style="0" width="3.51020408163265"/>
-    <col collapsed="false" hidden="false" max="1025" min="30" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12368,13 +12327,12 @@
   <dimension ref="A1:AC29"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AD1" activeCellId="0" sqref="AD1"/>
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="29" min="1" style="0" width="3.51020408163265"/>
-    <col collapsed="false" hidden="false" max="1025" min="30" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13463,7 +13421,6 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="29" min="1" style="0" width="3.51020408163265"/>
-    <col collapsed="false" hidden="false" max="1025" min="30" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14543,18 +14500,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.2040816326531"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.9285714285714"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>17</v>
       </c>
@@ -14576,8 +14537,97 @@
       <c r="G1" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="H1" s="0" t="s">
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="0" t="s">
         <v>23</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -14596,15 +14646,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Z25"/>
+  <dimension ref="A1:Z5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Y2" activeCellId="0" sqref="Y2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D19" activeCellId="0" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.3928571428571"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14612,214 +14662,62 @@
         <v>17</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="C1" s="6"/>
       <c r="Y1" s="0" t="s">
         <v>17</v>
       </c>
       <c r="Z1" s="0" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="B2" s="6"/>
+        <v>30</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>31</v>
+      </c>
       <c r="C2" s="6"/>
       <c r="Y2" s="0" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="B3" s="6"/>
+        <v>32</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>33</v>
+      </c>
       <c r="C3" s="6"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="6"/>
+      <c r="B4" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="C4" s="6"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="B5" s="6"/>
+        <v>35</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>36</v>
+      </c>
       <c r="C5" s="6"/>
     </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-    </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-    </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-    </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-    </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-    </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-    </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-    </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-    </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-    </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-    </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-    </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-    </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-    </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-    </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-    </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-    </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
-    </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="B23" s="6"/>
-      <c r="C23" s="6"/>
-    </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="B24" s="6"/>
-      <c r="C24" s="6"/>
-    </row>
-    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="B25" s="6"/>
-      <c r="C25" s="6"/>
-    </row>
   </sheetData>
-  <mergeCells count="25">
+  <mergeCells count="5">
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B25:C25"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -14839,13 +14737,12 @@
   <dimension ref="A1:AC29"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+      <selection pane="topLeft" activeCell="I24" activeCellId="0" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="29" min="1" style="0" width="3.51020408163265"/>
-    <col collapsed="false" hidden="false" max="1025" min="30" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15946,7 +15843,6 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="29" min="1" style="0" width="3.51020408163265"/>
-    <col collapsed="false" hidden="false" max="1025" min="30" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17035,7 +16931,6 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="29" min="1" style="0" width="3.51020408163265"/>
-    <col collapsed="false" hidden="false" max="1025" min="30" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18124,7 +18019,6 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="29" min="1" style="0" width="3.51020408163265"/>
-    <col collapsed="false" hidden="false" max="1025" min="30" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19213,7 +19107,6 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="29" min="1" style="0" width="3.51020408163265"/>
-    <col collapsed="false" hidden="false" max="1025" min="30" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20289,7 +20182,6 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="29" min="1" style="0" width="3.51020408163265"/>
-    <col collapsed="false" hidden="false" max="1025" min="30" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21378,7 +21270,6 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="29" min="1" style="0" width="3.51020408163265"/>
-    <col collapsed="false" hidden="false" max="1025" min="30" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Tallies logic + display Pair programming with @bradob98
</commit_message>
<xml_diff>
--- a/workbook/workbook.xlsx
+++ b/workbook/workbook.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" date1904="false" showObjects="all"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="1" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="993" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="993" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Week 1" r:id="rId2" sheetId="1" state="visible"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="39">
   <si>
     <t>Monday</t>
   </si>
@@ -73,9 +73,6 @@
     <t>CB</t>
   </si>
   <si>
-    <t>X</t>
-  </si>
-  <si>
     <t>S5</t>
   </si>
   <si>
@@ -98,6 +95,9 @@
   </si>
   <si>
     <t>S1</t>
+  </si>
+  <si>
+    <t>X</t>
   </si>
   <si>
     <t>I.D.</t>
@@ -282,14 +282,14 @@
   </sheetPr>
   <dimension ref="A1:AF29"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100">
-      <selection activeCell="R8" activeCellId="0" pane="topLeft" sqref="R8"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100">
+      <selection activeCell="F5" activeCellId="0" pane="topLeft" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="29" hidden="false" style="0" width="3.51020408163265" collapsed="true"/>
-    <col min="30" max="1025" hidden="false" style="0" width="8.50510204081633" collapsed="true"/>
+    <col min="30" max="1025" hidden="false" style="0" width="8.10204081632653" collapsed="true"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="1">
@@ -490,7 +490,7 @@
       <c r="AD4" s="5"/>
       <c r="AE4" s="5"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="5">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="5">
       <c r="A5" s="4" t="n">
         <v>1</v>
       </c>
@@ -499,19 +499,15 @@
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
-      <c r="E5" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4" t="s">
-        <v>10</v>
-      </c>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="G5" s="4"/>
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
-      <c r="K5" s="4" t="s">
-        <v>10</v>
-      </c>
+      <c r="K5" s="4"/>
       <c r="L5" s="4"/>
       <c r="M5" s="4"/>
       <c r="N5" s="4"/>
@@ -519,13 +515,11 @@
       <c r="P5" s="4"/>
       <c r="Q5" s="4"/>
       <c r="R5" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="S5" s="4"/>
       <c r="T5" s="4"/>
-      <c r="U5" s="4" t="s">
-        <v>10</v>
-      </c>
+      <c r="U5" s="4"/>
       <c r="V5" s="4"/>
       <c r="W5" s="4"/>
       <c r="X5" s="4"/>
@@ -542,7 +536,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -574,12 +568,12 @@
       <c r="AD6" s="5"/>
       <c r="AE6" s="5"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="7">
       <c r="A7" s="4" t="n">
         <v>3</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
@@ -590,19 +584,15 @@
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
       <c r="K7" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="L7" s="4"/>
-      <c r="M7" s="4" t="s">
-        <v>10</v>
-      </c>
+      <c r="M7" s="4"/>
       <c r="N7" s="4"/>
       <c r="O7" s="4"/>
       <c r="P7" s="4"/>
       <c r="Q7" s="4"/>
-      <c r="R7" s="4" t="s">
-        <v>10</v>
-      </c>
+      <c r="R7" s="4"/>
       <c r="S7" s="4"/>
       <c r="T7" s="4"/>
       <c r="U7" s="4"/>
@@ -617,21 +607,19 @@
       <c r="AD7" s="5"/>
       <c r="AE7" s="5"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="8">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="8">
       <c r="A8" s="4" t="n">
         <v>4</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
-      <c r="H8" s="4" t="s">
-        <v>10</v>
-      </c>
+      <c r="H8" s="4"/>
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
@@ -650,20 +638,18 @@
       <c r="X8" s="4"/>
       <c r="Y8" s="4"/>
       <c r="Z8" s="4"/>
-      <c r="AA8" s="4" t="s">
-        <v>10</v>
-      </c>
+      <c r="AA8" s="4"/>
       <c r="AB8" s="4"/>
       <c r="AC8" s="4"/>
       <c r="AD8" s="5"/>
       <c r="AE8" s="5"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="9">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="9">
       <c r="A9" s="4" t="n">
         <v>5</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
@@ -682,9 +668,7 @@
       <c r="Q9" s="4"/>
       <c r="R9" s="4"/>
       <c r="S9" s="4"/>
-      <c r="T9" s="4" t="s">
-        <v>10</v>
-      </c>
+      <c r="T9" s="4"/>
       <c r="U9" s="4"/>
       <c r="V9" s="4"/>
       <c r="W9" s="4"/>
@@ -1458,7 +1442,7 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="29" hidden="false" style="0" width="3.51020408163265" collapsed="true"/>
-    <col min="30" max="1025" hidden="false" style="0" width="8.50510204081633" collapsed="true"/>
+    <col min="30" max="1025" hidden="false" style="0" width="8.10204081632653" collapsed="true"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="1">
@@ -1661,7 +1645,7 @@
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
       <c r="E5" s="4" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
@@ -1693,7 +1677,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -1728,7 +1712,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
@@ -1763,7 +1747,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
@@ -1798,7 +1782,7 @@
         <v>5</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
@@ -2549,7 +2533,7 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="29" hidden="false" style="0" width="3.51020408163265" collapsed="true"/>
-    <col min="30" max="1025" hidden="false" style="0" width="8.50510204081633" collapsed="true"/>
+    <col min="30" max="1025" hidden="false" style="0" width="8.10204081632653" collapsed="true"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="1">
@@ -2782,7 +2766,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -2817,7 +2801,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
@@ -2852,7 +2836,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
@@ -2887,7 +2871,7 @@
         <v>5</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
@@ -3638,7 +3622,7 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="29" hidden="false" style="0" width="3.51020408163265" collapsed="true"/>
-    <col min="30" max="1025" hidden="false" style="0" width="8.50510204081633" collapsed="true"/>
+    <col min="30" max="1025" hidden="false" style="0" width="8.10204081632653" collapsed="true"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="1">
@@ -3871,7 +3855,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -3906,7 +3890,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
@@ -3941,7 +3925,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
@@ -3976,7 +3960,7 @@
         <v>5</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
@@ -4727,7 +4711,7 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="29" hidden="false" style="0" width="3.51020408163265" collapsed="true"/>
-    <col min="30" max="1025" hidden="false" style="0" width="8.50510204081633" collapsed="true"/>
+    <col min="30" max="1025" hidden="false" style="0" width="8.10204081632653" collapsed="true"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="1">
@@ -4960,7 +4944,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -4995,7 +4979,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
@@ -5030,7 +5014,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
@@ -5065,7 +5049,7 @@
         <v>5</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
@@ -5816,7 +5800,7 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="29" hidden="false" style="0" width="3.51020408163265" collapsed="true"/>
-    <col min="30" max="1025" hidden="false" style="0" width="8.50510204081633" collapsed="true"/>
+    <col min="30" max="1025" hidden="false" style="0" width="8.10204081632653" collapsed="true"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="1">
@@ -6049,7 +6033,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -6084,7 +6068,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
@@ -6119,7 +6103,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
@@ -6154,7 +6138,7 @@
         <v>5</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
@@ -6905,7 +6889,7 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="29" hidden="false" style="0" width="3.51020408163265" collapsed="true"/>
-    <col min="30" max="1025" hidden="false" style="0" width="8.50510204081633" collapsed="true"/>
+    <col min="30" max="1025" hidden="false" style="0" width="8.10204081632653" collapsed="true"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="1">
@@ -7138,7 +7122,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -7173,7 +7157,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
@@ -7208,7 +7192,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
@@ -7243,7 +7227,7 @@
         <v>5</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
@@ -7994,7 +7978,7 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="29" hidden="false" style="0" width="3.51020408163265" collapsed="true"/>
-    <col min="30" max="1025" hidden="false" style="0" width="8.50510204081633" collapsed="true"/>
+    <col min="30" max="1025" hidden="false" style="0" width="8.10204081632653" collapsed="true"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="1">
@@ -8227,7 +8211,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -8262,7 +8246,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
@@ -8297,7 +8281,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
@@ -8332,7 +8316,7 @@
         <v>5</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
@@ -9083,7 +9067,7 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="29" hidden="false" style="0" width="3.51020408163265" collapsed="true"/>
-    <col min="30" max="1025" hidden="false" style="0" width="8.50510204081633" collapsed="true"/>
+    <col min="30" max="1025" hidden="false" style="0" width="8.10204081632653" collapsed="true"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="1">
@@ -9316,7 +9300,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -9351,7 +9335,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
@@ -9386,7 +9370,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
@@ -9421,7 +9405,7 @@
         <v>5</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
@@ -10172,7 +10156,7 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="29" hidden="false" style="0" width="3.51020408163265" collapsed="true"/>
-    <col min="30" max="1025" hidden="false" style="0" width="8.50510204081633" collapsed="true"/>
+    <col min="30" max="1025" hidden="false" style="0" width="8.10204081632653" collapsed="true"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="1">
@@ -10405,7 +10389,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -10440,7 +10424,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
@@ -10475,7 +10459,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
@@ -10510,7 +10494,7 @@
         <v>5</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
@@ -11261,7 +11245,7 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="29" hidden="false" style="0" width="3.51020408163265" collapsed="true"/>
-    <col min="30" max="1025" hidden="false" style="0" width="8.50510204081633" collapsed="true"/>
+    <col min="30" max="1025" hidden="false" style="0" width="8.10204081632653" collapsed="true"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="1">
@@ -11494,7 +11478,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -11529,7 +11513,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
@@ -11564,7 +11548,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
@@ -11599,7 +11583,7 @@
         <v>5</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
@@ -12343,14 +12327,14 @@
   </sheetPr>
   <dimension ref="A1:AD29"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100">
-      <selection activeCell="AC9" activeCellId="0" pane="topLeft" sqref="AC9"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100">
+      <selection activeCell="F5" activeCellId="0" pane="topLeft" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="29" hidden="false" style="0" width="3.51020408163265" collapsed="true"/>
-    <col min="30" max="1025" hidden="false" style="0" width="8.50510204081633" collapsed="true"/>
+    <col min="30" max="1025" hidden="false" style="0" width="8.10204081632653" collapsed="true"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="1">
@@ -12554,7 +12538,7 @@
       <c r="D5" s="5"/>
       <c r="E5" s="4"/>
       <c r="F5" s="4" t="n">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
@@ -12562,7 +12546,7 @@
       <c r="J5" s="4"/>
       <c r="K5" s="4"/>
       <c r="L5" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M5" s="4"/>
       <c r="N5" s="4"/>
@@ -12587,7 +12571,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -12607,7 +12591,7 @@
       <c r="R6" s="4"/>
       <c r="S6" s="4"/>
       <c r="T6" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="U6" s="4"/>
       <c r="V6" s="4"/>
@@ -12624,7 +12608,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
@@ -12659,7 +12643,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
@@ -12670,10 +12654,10 @@
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
       <c r="K8" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L8" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M8" s="4"/>
       <c r="N8" s="4"/>
@@ -12698,7 +12682,7 @@
         <v>5</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
@@ -13449,7 +13433,7 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="29" hidden="false" style="0" width="3.51020408163265" collapsed="true"/>
-    <col min="30" max="1025" hidden="false" style="0" width="8.50510204081633" collapsed="true"/>
+    <col min="30" max="1025" hidden="false" style="0" width="8.10204081632653" collapsed="true"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="1">
@@ -13682,7 +13666,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -13717,7 +13701,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
@@ -13752,7 +13736,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
@@ -13787,7 +13771,7 @@
         <v>5</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
@@ -14532,18 +14516,18 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="D2" activeCellId="0" pane="topLeft" sqref="D2"/>
+      <selection activeCell="D6" activeCellId="0" pane="topLeft" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" hidden="false" style="0" width="8.50510204081633" collapsed="true"/>
-    <col min="3" max="3" hidden="false" style="0" width="12.4183673469388" collapsed="true"/>
-    <col min="4" max="4" hidden="false" style="0" width="10.2602040816327" collapsed="true"/>
-    <col min="5" max="5" hidden="false" style="0" width="11.8775510204082" collapsed="true"/>
-    <col min="6" max="6" hidden="false" style="0" width="10.3928571428571" collapsed="true"/>
-    <col min="7" max="7" hidden="false" style="0" width="14.8469387755102" collapsed="true"/>
-    <col min="8" max="1025" hidden="false" style="0" width="8.50510204081633" collapsed="true"/>
+    <col min="1" max="2" hidden="false" style="0" width="8.10204081632653" collapsed="true"/>
+    <col min="3" max="3" hidden="false" style="0" width="11.8775510204082" collapsed="true"/>
+    <col min="4" max="4" hidden="false" style="0" width="9.85204081632653" collapsed="true"/>
+    <col min="5" max="5" hidden="false" style="0" width="11.0714285714286" collapsed="true"/>
+    <col min="6" max="6" hidden="false" style="0" width="9.98979591836735" collapsed="true"/>
+    <col min="7" max="7" hidden="false" style="0" width="14.0408163265306" collapsed="true"/>
+    <col min="8" max="1025" hidden="false" style="0" width="8.10204081632653" collapsed="true"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="1">
@@ -14597,7 +14581,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>28</v>
@@ -14620,7 +14604,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>29</v>
@@ -14643,7 +14627,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>30</v>
@@ -14666,7 +14650,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>31</v>
@@ -14708,7 +14692,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1025" hidden="false" style="0" width="8.23469387755102" collapsed="true"/>
+    <col min="1" max="1025" hidden="false" style="0" width="8.50510204081633" collapsed="true"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="1">
@@ -14728,19 +14712,19 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="2">
       <c r="A2" s="0" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>33</v>
       </c>
       <c r="C2" s="6"/>
       <c r="Y2" s="0" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="3">
       <c r="A3" s="0" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>34</v>
@@ -14749,7 +14733,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="4">
       <c r="A4" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>35</v>
@@ -14767,7 +14751,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="6">
       <c r="A6" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B6" s="0" t="s">
         <v>38</v>
@@ -14805,7 +14789,7 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="29" hidden="false" style="0" width="3.51020408163265" collapsed="true"/>
-    <col min="30" max="1025" hidden="false" style="0" width="8.50510204081633" collapsed="true"/>
+    <col min="30" max="1025" hidden="false" style="0" width="8.10204081632653" collapsed="true"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="1">
@@ -15038,7 +15022,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -15073,7 +15057,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
@@ -15108,7 +15092,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
@@ -15143,7 +15127,7 @@
         <v>5</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
@@ -15894,7 +15878,7 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="29" hidden="false" style="0" width="3.51020408163265" collapsed="true"/>
-    <col min="30" max="1025" hidden="false" style="0" width="8.50510204081633" collapsed="true"/>
+    <col min="30" max="1025" hidden="false" style="0" width="8.10204081632653" collapsed="true"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="1">
@@ -16129,7 +16113,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -16164,7 +16148,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
@@ -16199,7 +16183,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
@@ -16234,7 +16218,7 @@
         <v>5</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
@@ -16985,7 +16969,7 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="29" hidden="false" style="0" width="3.51020408163265" collapsed="true"/>
-    <col min="30" max="1025" hidden="false" style="0" width="8.50510204081633" collapsed="true"/>
+    <col min="30" max="1025" hidden="false" style="0" width="8.10204081632653" collapsed="true"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="1">
@@ -17218,7 +17202,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -17253,7 +17237,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
@@ -17288,7 +17272,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
@@ -17323,7 +17307,7 @@
         <v>5</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
@@ -18074,7 +18058,7 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="29" hidden="false" style="0" width="3.51020408163265" collapsed="true"/>
-    <col min="30" max="1025" hidden="false" style="0" width="8.50510204081633" collapsed="true"/>
+    <col min="30" max="1025" hidden="false" style="0" width="8.10204081632653" collapsed="true"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="1">
@@ -18307,7 +18291,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -18342,7 +18326,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
@@ -18377,7 +18361,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
@@ -18412,7 +18396,7 @@
         <v>5</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
@@ -19163,7 +19147,7 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="29" hidden="false" style="0" width="3.51020408163265" collapsed="true"/>
-    <col min="30" max="1025" hidden="false" style="0" width="8.50510204081633" collapsed="true"/>
+    <col min="30" max="1025" hidden="false" style="0" width="8.10204081632653" collapsed="true"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="1">
@@ -19384,7 +19368,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -19419,7 +19403,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
@@ -19454,7 +19438,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
@@ -19489,7 +19473,7 @@
         <v>5</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
@@ -20239,7 +20223,7 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="29" hidden="false" style="0" width="3.51020408163265" collapsed="true"/>
-    <col min="30" max="1025" hidden="false" style="0" width="8.50510204081633" collapsed="true"/>
+    <col min="30" max="1025" hidden="false" style="0" width="8.10204081632653" collapsed="true"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="1">
@@ -20472,7 +20456,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -20507,7 +20491,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
@@ -20542,7 +20526,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
@@ -20577,7 +20561,7 @@
         <v>5</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
@@ -21328,7 +21312,7 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="29" hidden="false" style="0" width="3.51020408163265" collapsed="true"/>
-    <col min="30" max="1025" hidden="false" style="0" width="8.50510204081633" collapsed="true"/>
+    <col min="30" max="1025" hidden="false" style="0" width="8.10204081632653" collapsed="true"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="1">
@@ -21656,7 +21640,7 @@
         <v>2</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
@@ -21691,7 +21675,7 @@
         <v>3</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
@@ -21726,7 +21710,7 @@
         <v>4</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
@@ -21761,7 +21745,7 @@
         <v>5</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>

</xml_diff>